<commit_message>
Update in read row, column and cell
</commit_message>
<xml_diff>
--- a/ExcelApplicationScope_activity/resources/student.xlsx
+++ b/ExcelApplicationScope_activity/resources/student.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robots\UiPath-Tutorial\ExcelApplicationScope_activity\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPath\UiPath-Lessons\ExcelApplicationScope_activity\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00CA3D25-2D6B-47E3-96A8-3F82152C9E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1B61BC-5B58-4C2D-B179-70245F656A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="2580" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -124,13 +125,16 @@
     <t>Yi Wong</t>
   </si>
   <si>
+    <t>Rodriguez</t>
+  </si>
+  <si>
+    <t>Oceanography</t>
+  </si>
+  <si>
+    <t>Hello World</t>
+  </si>
+  <si>
     <t>Roll No.</t>
-  </si>
-  <si>
-    <t>Rodriguez</t>
-  </si>
-  <si>
-    <t>Oceanography</t>
   </si>
 </sst>
 </file>
@@ -522,12 +526,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394EE1C4-238C-4C22-BAF7-25A707A682BF}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069642E0-99DD-4BBE-8800-7BE560955280}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -538,7 +569,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -588,10 +619,10 @@
         <v>1024</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="D3" s="2">
         <v>19</v>
@@ -917,6 +948,11 @@
       <c r="G16" s="7">
         <f t="shared" si="0"/>
         <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>